<commit_message>
authenticator codes are added
</commit_message>
<xml_diff>
--- a/TestData/RestAssuredTestData.xlsx
+++ b/TestData/RestAssuredTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>TestName</t>
   </si>
@@ -74,6 +74,15 @@
   </si>
   <si>
     <t>TC002_GET_F1_Driver</t>
+  </si>
+  <si>
+    <t>AuthenticationParameter</t>
+  </si>
+  <si>
+    <t>PreemptiveBasicAuthScheme</t>
+  </si>
+  <si>
+    <t>Username_ToolsQA:Password_TestPassword</t>
   </si>
 </sst>
 </file>
@@ -461,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -475,13 +484,14 @@
     <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="48.28515625" customWidth="1"/>
+    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="48.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -501,19 +511,22 @@
         <v>5</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="75">
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="75">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -529,17 +542,22 @@
       <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="F2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3"/>
+      <c r="K2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="75">
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="75">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -557,23 +575,24 @@
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3"/>
+      <c r="K3" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1"/>
-    <row r="5" spans="1:10" s="2" customFormat="1"/>
-    <row r="6" spans="1:10" s="2" customFormat="1"/>
-    <row r="7" spans="1:10" s="2" customFormat="1"/>
-    <row r="8" spans="1:10" s="2" customFormat="1"/>
-    <row r="9" spans="1:10" s="2" customFormat="1"/>
-    <row r="10" spans="1:10" s="2" customFormat="1"/>
-    <row r="11" spans="1:10" s="2" customFormat="1"/>
-    <row r="12" spans="1:10" s="2" customFormat="1"/>
+    <row r="4" spans="1:11" s="2" customFormat="1"/>
+    <row r="5" spans="1:11" s="2" customFormat="1"/>
+    <row r="6" spans="1:11" s="2" customFormat="1"/>
+    <row r="7" spans="1:11" s="2" customFormat="1"/>
+    <row r="8" spans="1:11" s="2" customFormat="1"/>
+    <row r="9" spans="1:11" s="2" customFormat="1"/>
+    <row r="10" spans="1:11" s="2" customFormat="1"/>
+    <row r="11" spans="1:11" s="2" customFormat="1"/>
+    <row r="12" spans="1:11" s="2" customFormat="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>

</xml_diff>